<commit_message>
Plot true values on map
</commit_message>
<xml_diff>
--- a/Prediction_ANN/Prediction_ANN/predicted.xlsx
+++ b/Prediction_ANN/Prediction_ANN/predicted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Documents\GitHub\Prediction_ANN\Prediction_ANN\Prediction_ANN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2293FC-E74F-4B92-8CA6-F7DB9C037871}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44548CEA-E6FF-44C2-B42E-05B3160276DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="345" windowWidth="25395" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>lat</t>
   </si>
   <si>
-    <t>lon</t>
-  </si>
-  <si>
     <t>true values</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>0.006094916360080242</t>
+  </si>
+  <si>
+    <t>lng</t>
   </si>
 </sst>
 </file>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1114" workbookViewId="0">
-      <selection activeCell="H1156" sqref="H1156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,13 +457,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -20166,7 +20166,7 @@
         <v>-6.4000000000000003E-3</v>
       </c>
       <c r="E1160" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>